<commit_message>
this file will not be further updated as linux academy courses has been moved to acloud.guru.
</commit_message>
<xml_diff>
--- a/Linux Academy Course Schedule.xlsx
+++ b/Linux Academy Course Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD66E31-BB6D-48E0-AD12-563F05A19C9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B43A5E7-CDDA-4F71-A358-E2B8712E36D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{774EDFFE-DF12-4610-BDB7-181FB7FCF003}"/>
   </bookViews>
@@ -207,9 +207,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>https://linuxacademy.com/cp/coursescheduler/view/id/490334</t>
-  </si>
-  <si>
     <t>https://linuxacademy.com/cp/coursescheduler/view/id/490335</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>https://linuxacademy.com/cp/coursescheduler/view/id/495697</t>
+  </si>
+  <si>
+    <t>https://linuxacademy.com/cp/coursescheduler/view/id/501905</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9A495D-E1E3-4D0C-8FC5-1EEC5E37F3D1}">
   <dimension ref="A1:F272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
@@ -1019,7 +1019,7 @@
         <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
         <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
@@ -1152,7 +1152,7 @@
         <v>10</v>
       </c>
       <c r="F65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>16</v>
       </c>
       <c r="F79" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
@@ -1239,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.3">
@@ -1308,7 +1308,7 @@
         <v>15</v>
       </c>
       <c r="E93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.3">
@@ -1352,7 +1352,7 @@
         <v>22</v>
       </c>
       <c r="E100" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.3">
@@ -1395,7 +1395,7 @@
         <v>30</v>
       </c>
       <c r="E108" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.3">
@@ -1455,9 +1455,6 @@
       <c r="C120">
         <v>9</v>
       </c>
-      <c r="E120" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C121">
@@ -1516,9 +1513,6 @@
       <c r="C131">
         <v>20</v>
       </c>
-      <c r="E131" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C132">
@@ -1534,6 +1528,9 @@
       <c r="C134">
         <v>23</v>
       </c>
+      <c r="E134" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C135">
@@ -1555,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="E138" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
@@ -1583,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F144" t="s">
         <v>4</v>
@@ -1598,6 +1595,9 @@
       <c r="C146">
         <v>3</v>
       </c>
+      <c r="E146" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="147" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C147">
@@ -1628,9 +1628,6 @@
       <c r="C152">
         <v>9</v>
       </c>
-      <c r="E152" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="153" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C153">
@@ -1671,81 +1668,84 @@
       <c r="C160">
         <v>17</v>
       </c>
-      <c r="E160" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C161">
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C162">
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C163">
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C164">
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C165">
         <v>22</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C166">
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C167">
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C168">
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C169">
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C170">
         <v>27</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C171">
         <v>28</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C172">
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C173">
         <v>30</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C174">
         <v>31</v>
       </c>
-    </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E174" t="s">
+        <v>87</v>
+      </c>
+      <c r="F174" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>56</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="E177" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="178" spans="3:5" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
         <v>15</v>
       </c>
       <c r="E191" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="3:5" x14ac:dyDescent="0.3">
@@ -1879,7 +1879,7 @@
         <v>24</v>
       </c>
       <c r="E200" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="201" spans="2:5" x14ac:dyDescent="0.3">
@@ -1937,7 +1937,7 @@
         <v>4</v>
       </c>
       <c r="E212" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="213" spans="3:5" x14ac:dyDescent="0.3">
@@ -1945,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="E213" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="214" spans="3:5" x14ac:dyDescent="0.3">
@@ -2023,7 +2023,7 @@
         <v>20</v>
       </c>
       <c r="E228" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="229" spans="3:5" x14ac:dyDescent="0.3">
@@ -2056,7 +2056,7 @@
         <v>26</v>
       </c>
       <c r="E234" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="235" spans="3:5" x14ac:dyDescent="0.3">
@@ -2074,7 +2074,7 @@
         <v>29</v>
       </c>
       <c r="E237" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="238" spans="3:5" x14ac:dyDescent="0.3">
@@ -2142,7 +2142,7 @@
         <v>10</v>
       </c>
       <c r="E251" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.3">
@@ -2274,7 +2274,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2322,7 +2322,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2592,10 +2592,10 @@
     </row>
     <row r="19" spans="2:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>